<commit_message>
fix bug di import init pake sample number
</commit_message>
<xml_diff>
--- a/storage/app/public/form_import/form_import_init.xlsx
+++ b/storage/app/public/form_import/form_import_init.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aldhi/Documents/Storage/Dev/laravel/08-socfin-sawit/storage/app/public/form_import/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04E0D2B6-5913-DC45-B9E3-6EF4B4F27893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75796D0A-4CE0-5E4F-BD8F-20F7222A9E7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17520" yWindow="31260" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,10 +41,10 @@
     <t>&lt;end&gt;</t>
   </si>
   <si>
-    <t>Sample ID</t>
+    <t>Tgl Initiation</t>
   </si>
   <si>
-    <t>Tgl Initiation</t>
+    <t>Sample Number</t>
   </si>
 </sst>
 </file>
@@ -433,21 +433,21 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>